<commit_message>
Updating a few files with new info!
</commit_message>
<xml_diff>
--- a/vars_forexpt/heattol_vars.xlsx
+++ b/vars_forexpt/heattol_vars.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="13260" yWindow="0" windowWidth="35220" windowHeight="21020" tabRatio="500" activeTab="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="210">
   <si>
     <t>File started on 26 July 2016</t>
   </si>
@@ -643,6 +643,18 @@
   </si>
   <si>
     <t>Alicante bouchet</t>
+  </si>
+  <si>
+    <t>On 21 November 2016:</t>
+  </si>
+  <si>
+    <t>Lizzie updated this file to pick which plants to keep. She aimed for a mix of colors and phenophases from plants where at least some individuals flowered! (SeeVitisExpReps.xlsx)</t>
+  </si>
+  <si>
+    <t>Keep! For possible future experiments (21 Nov 2016):</t>
+  </si>
+  <si>
+    <t>Reps total</t>
   </si>
 </sst>
 </file>
@@ -738,8 +750,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="273">
+  <cellStyleXfs count="281">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1027,7 +1047,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="273">
+  <cellStyles count="281">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1164,6 +1184,10 @@
     <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1300,6 +1324,10 @@
     <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1629,10 +1657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1769,6 +1797,16 @@
     <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>199</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="B29" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -1783,10 +1821,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X44"/>
+  <dimension ref="A1:X57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="D12" workbookViewId="0">
+      <selection activeCell="R58" sqref="R58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3446,6 +3484,127 @@
       </c>
       <c r="R44" t="s">
         <v>203</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18">
+      <c r="M47" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18">
+      <c r="R48" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="49" spans="13:18">
+      <c r="M49" t="s">
+        <v>105</v>
+      </c>
+      <c r="P49" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>131</v>
+      </c>
+      <c r="R49">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="13:18">
+      <c r="M50" t="s">
+        <v>4</v>
+      </c>
+      <c r="N50" t="s">
+        <v>159</v>
+      </c>
+      <c r="P50" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>131</v>
+      </c>
+      <c r="R50">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="13:18">
+      <c r="M51" t="s">
+        <v>19</v>
+      </c>
+      <c r="N51" t="s">
+        <v>159</v>
+      </c>
+      <c r="P51" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>131</v>
+      </c>
+      <c r="R51">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="13:18">
+      <c r="M52" t="s">
+        <v>69</v>
+      </c>
+      <c r="P52" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>131</v>
+      </c>
+      <c r="R52">
+        <f>7+6</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="13:18">
+      <c r="M53" t="s">
+        <v>127</v>
+      </c>
+      <c r="P53" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>131</v>
+      </c>
+      <c r="R53">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="13:18">
+      <c r="M54" t="s">
+        <v>45</v>
+      </c>
+      <c r="P54" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>134</v>
+      </c>
+      <c r="R54">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="13:18">
+      <c r="M55" t="s">
+        <v>83</v>
+      </c>
+      <c r="P55" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>134</v>
+      </c>
+      <c r="R55">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="13:18">
+      <c r="R57">
+        <f>SUM(R49:R55)</f>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>